<commit_message>
Added column colour for easy understanding on change %
</commit_message>
<xml_diff>
--- a/nifty50_latest_snapshot.xlsx
+++ b/nifty50_latest_snapshot.xlsx
@@ -26,12 +26,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C6EFCE"/>
+        <bgColor rgb="00C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFC7CE"/>
+        <bgColor rgb="00FFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,8 +58,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -589,7 +603,7 @@
       <c r="C2" t="n">
         <v>1274.5</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2" s="1" t="n">
         <v>2.77</v>
       </c>
     </row>
@@ -605,7 +619,7 @@
       <c r="C3" t="n">
         <v>3298.9</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3" s="1" t="n">
         <v>1.65</v>
       </c>
     </row>
@@ -621,7 +635,7 @@
       <c r="C4" t="n">
         <v>1906.7</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4" s="1" t="n">
         <v>1.31</v>
       </c>
     </row>
@@ -637,7 +651,7 @@
       <c r="C5" t="n">
         <v>1889.1</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5" s="1" t="n">
         <v>3</v>
       </c>
     </row>
@@ -653,7 +667,7 @@
       <c r="C6" t="n">
         <v>1406.7</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6" s="1" t="n">
         <v>3.28</v>
       </c>
     </row>
@@ -669,7 +683,7 @@
       <c r="C7" t="n">
         <v>2375</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7" s="1" t="n">
         <v>0.76</v>
       </c>
     </row>
@@ -685,7 +699,7 @@
       <c r="C8" t="n">
         <v>1419.5</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8" s="1" t="n">
         <v>1.54</v>
       </c>
     </row>
@@ -701,7 +715,7 @@
       <c r="C9" t="n">
         <v>797.45</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9" s="1" t="n">
         <v>3.3</v>
       </c>
     </row>
@@ -717,7 +731,7 @@
       <c r="C10" t="n">
         <v>2188.1</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D10" s="1" t="n">
         <v>3.46</v>
       </c>
     </row>
@@ -733,7 +747,7 @@
       <c r="C11" t="n">
         <v>427.25</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D11" s="1" t="n">
         <v>0.53</v>
       </c>
     </row>
@@ -749,7 +763,7 @@
       <c r="C12" t="n">
         <v>1751.5</v>
       </c>
-      <c r="D12" t="n">
+      <c r="D12" s="1" t="n">
         <v>3.33</v>
       </c>
     </row>
@@ -765,7 +779,7 @@
       <c r="C13" t="n">
         <v>3247.3</v>
       </c>
-      <c r="D13" t="n">
+      <c r="D13" s="1" t="n">
         <v>1.03</v>
       </c>
     </row>
@@ -781,7 +795,7 @@
       <c r="C14" t="n">
         <v>9162.5</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D14" s="1" t="n">
         <v>1.36</v>
       </c>
     </row>
@@ -797,7 +811,7 @@
       <c r="C15" t="n">
         <v>1438</v>
       </c>
-      <c r="D15" t="n">
+      <c r="D15" s="1" t="n">
         <v>1.27</v>
       </c>
     </row>
@@ -813,7 +827,7 @@
       <c r="C16" t="n">
         <v>11695</v>
       </c>
-      <c r="D16" t="n">
+      <c r="D16" s="1" t="n">
         <v>0.27</v>
       </c>
     </row>
@@ -829,7 +843,7 @@
       <c r="C17" t="n">
         <v>364</v>
       </c>
-      <c r="D17" t="n">
+      <c r="D17" s="1" t="n">
         <v>1.32</v>
       </c>
     </row>
@@ -845,7 +859,7 @@
       <c r="C18" t="n">
         <v>11901</v>
       </c>
-      <c r="D18" t="n">
+      <c r="D18" s="1" t="n">
         <v>2.01</v>
       </c>
     </row>
@@ -861,7 +875,7 @@
       <c r="C19" t="n">
         <v>1190.8</v>
       </c>
-      <c r="D19" t="n">
+      <c r="D19" s="1" t="n">
         <v>3.05</v>
       </c>
     </row>
@@ -877,7 +891,7 @@
       <c r="C20" t="n">
         <v>2679.4</v>
       </c>
-      <c r="D20" t="n">
+      <c r="D20" s="1" t="n">
         <v>1.8</v>
       </c>
     </row>
@@ -893,7 +907,7 @@
       <c r="C21" t="n">
         <v>2035.3</v>
       </c>
-      <c r="D21" t="n">
+      <c r="D21" s="1" t="n">
         <v>3.76</v>
       </c>
     </row>
@@ -909,7 +923,7 @@
       <c r="C22" t="n">
         <v>243.49</v>
       </c>
-      <c r="D22" t="n">
+      <c r="D22" s="1" t="n">
         <v>1.03</v>
       </c>
     </row>
@@ -925,7 +939,7 @@
       <c r="C23" t="n">
         <v>3327.5</v>
       </c>
-      <c r="D23" t="n">
+      <c r="D23" s="1" t="n">
         <v>2.38</v>
       </c>
     </row>
@@ -941,7 +955,7 @@
       <c r="C24" t="n">
         <v>309</v>
       </c>
-      <c r="D24" t="n">
+      <c r="D24" s="1" t="n">
         <v>1.16</v>
       </c>
     </row>
@@ -957,7 +971,7 @@
       <c r="C25" t="n">
         <v>1259.4</v>
       </c>
-      <c r="D25" t="n">
+      <c r="D25" s="1" t="n">
         <v>2.15</v>
       </c>
     </row>
@@ -989,7 +1003,7 @@
       <c r="C27" t="n">
         <v>236.9</v>
       </c>
-      <c r="D27" t="n">
+      <c r="D27" s="1" t="n">
         <v>0.8100000000000001</v>
       </c>
     </row>
@@ -1005,7 +1019,7 @@
       <c r="C28" t="n">
         <v>1007.2</v>
       </c>
-      <c r="D28" t="n">
+      <c r="D28" s="1" t="n">
         <v>1.12</v>
       </c>
     </row>
@@ -1021,7 +1035,7 @@
       <c r="C29" t="n">
         <v>2467.9</v>
       </c>
-      <c r="D29" t="n">
+      <c r="D29" s="1" t="n">
         <v>0.33</v>
       </c>
     </row>
@@ -1037,7 +1051,7 @@
       <c r="C30" t="n">
         <v>398.85</v>
       </c>
-      <c r="D30" t="n">
+      <c r="D30" s="1" t="n">
         <v>0.49</v>
       </c>
     </row>
@@ -1053,7 +1067,7 @@
       <c r="C31" t="n">
         <v>2416.6</v>
       </c>
-      <c r="D31" t="n">
+      <c r="D31" s="1" t="n">
         <v>1.88</v>
       </c>
     </row>
@@ -1069,7 +1083,7 @@
       <c r="C32" t="n">
         <v>621.55</v>
       </c>
-      <c r="D32" t="n">
+      <c r="D32" s="1" t="n">
         <v>0.89</v>
       </c>
     </row>
@@ -1085,7 +1099,7 @@
       <c r="C33" t="n">
         <v>8018</v>
       </c>
-      <c r="D33" t="n">
+      <c r="D33" s="1" t="n">
         <v>0.3</v>
       </c>
     </row>
@@ -1101,7 +1115,7 @@
       <c r="C34" t="n">
         <v>2760.7</v>
       </c>
-      <c r="D34" t="n">
+      <c r="D34" s="1" t="n">
         <v>2.21</v>
       </c>
     </row>
@@ -1117,7 +1131,7 @@
       <c r="C35" t="n">
         <v>5130.5</v>
       </c>
-      <c r="D35" t="n">
+      <c r="D35" s="1" t="n">
         <v>1.55</v>
       </c>
     </row>
@@ -1133,7 +1147,7 @@
       <c r="C36" t="n">
         <v>1608.2</v>
       </c>
-      <c r="D36" t="n">
+      <c r="D36" s="1" t="n">
         <v>3.22</v>
       </c>
     </row>
@@ -1149,7 +1163,7 @@
       <c r="C37" t="n">
         <v>137.14</v>
       </c>
-      <c r="D37" t="n">
+      <c r="D37" s="1" t="n">
         <v>2.04</v>
       </c>
     </row>
@@ -1165,7 +1179,7 @@
       <c r="C38" t="n">
         <v>5678.5</v>
       </c>
-      <c r="D38" t="n">
+      <c r="D38" s="1" t="n">
         <v>1.12</v>
       </c>
     </row>
@@ -1181,7 +1195,7 @@
       <c r="C39" t="n">
         <v>720.05</v>
       </c>
-      <c r="D39" t="n">
+      <c r="D39" s="1" t="n">
         <v>0.5600000000000001</v>
       </c>
     </row>
@@ -1197,7 +1211,7 @@
       <c r="C40" t="n">
         <v>295.15</v>
       </c>
-      <c r="D40" t="n">
+      <c r="D40" s="1" t="n">
         <v>0.73</v>
       </c>
     </row>
@@ -1213,7 +1227,7 @@
       <c r="C41" t="n">
         <v>3771.8</v>
       </c>
-      <c r="D41" t="n">
+      <c r="D41" s="2" t="n">
         <v>-0.27</v>
       </c>
     </row>
@@ -1229,7 +1243,7 @@
       <c r="C42" t="n">
         <v>1306.8</v>
       </c>
-      <c r="D42" t="n">
+      <c r="D42" s="1" t="n">
         <v>0.9</v>
       </c>
     </row>
@@ -1245,7 +1259,7 @@
       <c r="C43" t="n">
         <v>609.5</v>
       </c>
-      <c r="D43" t="n">
+      <c r="D43" s="1" t="n">
         <v>0.1</v>
       </c>
     </row>
@@ -1261,7 +1275,7 @@
       <c r="C44" t="n">
         <v>691.75</v>
       </c>
-      <c r="D44" t="n">
+      <c r="D44" s="1" t="n">
         <v>2.18</v>
       </c>
     </row>
@@ -1277,7 +1291,7 @@
       <c r="C45" t="n">
         <v>1120.2</v>
       </c>
-      <c r="D45" t="n">
+      <c r="D45" s="1" t="n">
         <v>1.47</v>
       </c>
     </row>
@@ -1293,7 +1307,7 @@
       <c r="C46" t="n">
         <v>7073.5</v>
       </c>
-      <c r="D46" t="n">
+      <c r="D46" s="1" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -1309,7 +1323,7 @@
       <c r="C47" t="n">
         <v>1163.6</v>
       </c>
-      <c r="D47" t="n">
+      <c r="D47" s="1" t="n">
         <v>1.17</v>
       </c>
     </row>
@@ -1325,7 +1339,7 @@
       <c r="C48" t="n">
         <v>1515.2</v>
       </c>
-      <c r="D48" t="n">
+      <c r="D48" s="1" t="n">
         <v>1.15</v>
       </c>
     </row>
@@ -1341,7 +1355,7 @@
       <c r="C49" t="n">
         <v>246.47</v>
       </c>
-      <c r="D49" t="n">
+      <c r="D49" s="1" t="n">
         <v>1.45</v>
       </c>
     </row>
@@ -1357,7 +1371,7 @@
       <c r="C50" t="n">
         <v>794.7</v>
       </c>
-      <c r="D50" t="n">
+      <c r="D50" s="1" t="n">
         <v>0.82</v>
       </c>
     </row>

</xml_diff>